<commit_message>
ajustes no painel de controle
</commit_message>
<xml_diff>
--- a/Organização Geral.xlsx
+++ b/Organização Geral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e9d47a71a04e5b6/Documentos/Coisas do Pedro Lindo/GitHub/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3F4B47EB-367A-4203-ACE0-0EDFFC5FD1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B9DDA2D-BD25-463F-A40B-E157E5D4B87C}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{3F4B47EB-367A-4203-ACE0-0EDFFC5FD1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BD7D75B-376D-4725-A211-1BB001BB1247}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="2565" windowWidth="18000" windowHeight="9360" xr2:uid="{72021B9B-4A70-425A-94EB-D0FDB5FE6FE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{72021B9B-4A70-425A-94EB-D0FDB5FE6FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendário do técnico" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t xml:space="preserve">Segunda </t>
   </si>
@@ -149,9 +149,6 @@
 visualizar publi. e excluir</t>
   </si>
   <si>
-    <t>Fazer BD do trabalho POO</t>
-  </si>
-  <si>
     <t>Fazer a pesquisa por data
 e a pesquisa no index</t>
   </si>
@@ -159,12 +156,6 @@
     <t>Feriado</t>
   </si>
   <si>
-    <t>Fazer coisas pendentes</t>
-  </si>
-  <si>
-    <t>Fazer Coisas Pendentes</t>
-  </si>
-  <si>
     <t>Sab.</t>
   </si>
   <si>
@@ -175,9 +166,6 @@
 REACT</t>
   </si>
   <si>
-    <t>Comentários</t>
-  </si>
-  <si>
     <t>Postagem + 
 comentários</t>
   </si>
@@ -198,6 +186,24 @@
   </si>
   <si>
     <t>Terminar Navegação // e iniciar o salvamento de dados</t>
+  </si>
+  <si>
+    <t>Terminar menu POO + Banco de dados</t>
+  </si>
+  <si>
+    <t>Fazer UI do Painel de Controle</t>
+  </si>
+  <si>
+    <t>Fazer Slides do TCC</t>
+  </si>
+  <si>
+    <t>Preparar apresentação</t>
+  </si>
+  <si>
+    <t>Comentários Mobile</t>
+  </si>
+  <si>
+    <t>Integrar as telas</t>
   </si>
 </sst>
 </file>
@@ -249,196 +255,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-416]d\-mmm;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <font>
         <b val="0"/>
@@ -469,11 +286,264 @@
       <font>
         <b val="0"/>
         <i/>
+        <color theme="1"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-416]d\-mmm;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -491,28 +561,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B63BDC07-4760-4060-B9ED-33FF3571D692}" name="Tabela3" displayName="Tabela3" ref="G4:Y10" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B63BDC07-4760-4060-B9ED-33FF3571D692}" name="Tabela3" displayName="Tabela3" ref="G4:Y10" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="G4:Y10" xr:uid="{B63BDC07-4760-4060-B9ED-33FF3571D692}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{3AA79EB4-57A3-4B5F-A8AF-0112FB613DAD}" name="13-jun" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{AC154EE8-5922-4756-8844-67F4E92E74E2}" name="14-jun" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{C198B889-7519-47AF-895F-1C44454311EE}" name="15-jun" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{10845774-9AE7-45A0-972E-E4A4D0300756}" name="16-jun" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{3623D879-D926-4F3E-B65A-B5530192F4C2}" name="17-jun" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{D95CD071-9A1D-4767-A50F-F78CCA1D7C50}" name="18-jun" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{F62D3B69-7501-4C6A-9AA2-D9AEEAB679C6}" name="19-jun" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{DEA6AD96-7E2F-469C-92A5-A2C937CC84FD}" name="20-jun" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{98AFA71A-FBFF-4BF8-A739-3FABEB784F60}" name="21-jun" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{5AFA6BBB-214F-4CE8-A7BC-757DBCE5E0CF}" name="22-jun" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{446705AE-E189-4FB5-A37B-0D69BEECC996}" name="23-jun" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{0FCD6266-EBD1-4459-B6F8-F142A471C411}" name="24-jun" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{B83DD26E-9E47-4869-AFFE-5FFB3B7980DD}" name="25-jun" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{46440F7E-A9F3-45A8-9936-28E3F8EAEFF3}" name="26-jun" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{9A55DC73-B474-4BF1-8732-7D5C8CB56620}" name="27-jun" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{0FDCF250-3C5E-43F2-8025-F499B4F4161C}" name="28-jun" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{90BD5B0A-2B52-4990-BAEA-5EC1E5ADC2B2}" name="29-jun" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{FDB9A6AD-9082-44E9-A741-8311BF2C0C38}" name="30-jun" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{F4A471A9-0941-4B1C-BC3E-55D8376CF154}" name="1-jul" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3AA79EB4-57A3-4B5F-A8AF-0112FB613DAD}" name="13-jun" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{AC154EE8-5922-4756-8844-67F4E92E74E2}" name="14-jun" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{C198B889-7519-47AF-895F-1C44454311EE}" name="15-jun" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{10845774-9AE7-45A0-972E-E4A4D0300756}" name="16-jun" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{3623D879-D926-4F3E-B65A-B5530192F4C2}" name="17-jun" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{D95CD071-9A1D-4767-A50F-F78CCA1D7C50}" name="18-jun" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{F62D3B69-7501-4C6A-9AA2-D9AEEAB679C6}" name="19-jun" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{DEA6AD96-7E2F-469C-92A5-A2C937CC84FD}" name="20-jun" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{98AFA71A-FBFF-4BF8-A739-3FABEB784F60}" name="21-jun" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{5AFA6BBB-214F-4CE8-A7BC-757DBCE5E0CF}" name="22-jun" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{446705AE-E189-4FB5-A37B-0D69BEECC996}" name="23-jun" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{0FCD6266-EBD1-4459-B6F8-F142A471C411}" name="24-jun" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{B83DD26E-9E47-4869-AFFE-5FFB3B7980DD}" name="25-jun" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{46440F7E-A9F3-45A8-9936-28E3F8EAEFF3}" name="26-jun" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{9A55DC73-B474-4BF1-8732-7D5C8CB56620}" name="27-jun" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{0FDCF250-3C5E-43F2-8025-F499B4F4161C}" name="28-jun" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{90BD5B0A-2B52-4990-BAEA-5EC1E5ADC2B2}" name="29-jun" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{FDB9A6AD-9082-44E9-A741-8311BF2C0C38}" name="30-jun" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{F4A471A9-0941-4B1C-BC3E-55D8376CF154}" name="1-jul" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -817,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41B0F22-50C8-45B6-9ED7-43F6C5E47FD7}">
   <dimension ref="G4:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,16 +1031,16 @@
         <v>5</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="M6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>10</v>
@@ -988,10 +1058,10 @@
         <v>8</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>10</v>
@@ -1011,10 +1081,10 @@
     </row>
     <row r="7" spans="7:25" ht="45" x14ac:dyDescent="0.25">
       <c r="G7" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>6</v>
@@ -1024,29 +1094,27 @@
         <v>8</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="S7" s="2"/>
       <c r="T7" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>14</v>
@@ -1054,9 +1122,7 @@
       <c r="V7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="W7" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2" t="s">
         <v>15</v>
@@ -1073,23 +1139,29 @@
         <v>9</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="3"/>
+      <c r="P8" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="Q8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="V8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1100,7 +1172,7 @@
     <row r="9" spans="7:25" ht="30" x14ac:dyDescent="0.25">
       <c r="G9" s="3"/>
       <c r="H9" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -1132,7 +1204,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1156,17 +1228,17 @@
     <row r="15" spans="7:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="P15">
-    <cfRule type="timePeriod" dxfId="23" priority="3" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="7" priority="3" timePeriod="yesterday">
       <formula>FLOOR(P15,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4 I4:Y4 L7:Y9 G5:Y6 G7:J9">
-    <cfRule type="timePeriod" dxfId="22" priority="2" timePeriod="yesterday">
+  <conditionalFormatting sqref="G4 I4:Y4 L9:Y9 G5:Y6 G7:J9 L7:O8 Q7:Y8">
+    <cfRule type="timePeriod" dxfId="6" priority="2" timePeriod="yesterday">
       <formula>FLOOR(G4,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:K10">
-    <cfRule type="timePeriod" dxfId="21" priority="1" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="5" priority="1" timePeriod="yesterday">
       <formula>FLOOR(K7,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>